<commit_message>
Backend node and attack data sheet updates
</commit_message>
<xml_diff>
--- a/static/sample/sna/Iranian_Influence.xlsx
+++ b/static/sample/sna/Iranian_Influence.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxer\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="84" documentId="1E364893CC8683BBAC371AEE5BC262997293FAB9" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{D925E690-E9C7-432C-9E2A-DA37427ADFD1}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11460" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Node Sheet" sheetId="4" r:id="rId1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="118">
   <si>
     <t>ID</t>
   </si>
@@ -293,7 +292,16 @@
     <t>Independent</t>
   </si>
   <si>
-    <t>Revisionist</t>
+    <t>Al-Qaeda</t>
+  </si>
+  <si>
+    <t>Mukhtar Army</t>
+  </si>
+  <si>
+    <t>Al-Naqshabandiya Army</t>
+  </si>
+  <si>
+    <t>Military Council of the Tribal Revolutionaries</t>
   </si>
   <si>
     <t>Name</t>
@@ -372,7 +380,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -754,16 +762,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:X43"/>
+  <dimension ref="A1:X35"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{51F8DEE0-4D01-5F28-A812-FC0BD7CAC4A5}">
-      <pane ySplit="1" topLeftCell="B2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
@@ -773,7 +781,7 @@
     <col min="9" max="9" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="12.75">
+    <row r="1" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -837,7 +845,7 @@
       <c r="W1" s="3"/>
       <c r="X1" s="3"/>
     </row>
-    <row r="2" spans="1:24" ht="12.75">
+    <row r="2" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -889,7 +897,7 @@
       <c r="W2" s="3"/>
       <c r="X2" s="3"/>
     </row>
-    <row r="3" spans="1:24" ht="12.75">
+    <row r="3" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>20</v>
       </c>
@@ -937,7 +945,7 @@
       <c r="W3" s="3"/>
       <c r="X3" s="3"/>
     </row>
-    <row r="4" spans="1:24" ht="12.75">
+    <row r="4" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>24</v>
       </c>
@@ -993,7 +1001,7 @@
       <c r="W4" s="3"/>
       <c r="X4" s="3"/>
     </row>
-    <row r="5" spans="1:24" ht="12.75">
+    <row r="5" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>30</v>
       </c>
@@ -1041,7 +1049,7 @@
       <c r="W5" s="3"/>
       <c r="X5" s="3"/>
     </row>
-    <row r="6" spans="1:24" ht="12.75">
+    <row r="6" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>34</v>
       </c>
@@ -1087,7 +1095,7 @@
       <c r="W6" s="3"/>
       <c r="X6" s="3"/>
     </row>
-    <row r="7" spans="1:24" ht="12.75">
+    <row r="7" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>37</v>
       </c>
@@ -1135,7 +1143,7 @@
       <c r="W7" s="3"/>
       <c r="X7" s="3"/>
     </row>
-    <row r="8" spans="1:24" ht="12.75">
+    <row r="8" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>40</v>
       </c>
@@ -1193,7 +1201,7 @@
       <c r="W8" s="3"/>
       <c r="X8" s="3"/>
     </row>
-    <row r="9" spans="1:24" ht="12.75">
+    <row r="9" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>45</v>
       </c>
@@ -1251,7 +1259,7 @@
       <c r="W9" s="3"/>
       <c r="X9" s="3"/>
     </row>
-    <row r="10" spans="1:24" ht="12.75">
+    <row r="10" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>32</v>
       </c>
@@ -1303,7 +1311,7 @@
       <c r="W10" s="3"/>
       <c r="X10" s="3"/>
     </row>
-    <row r="11" spans="1:24" ht="12.75">
+    <row r="11" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>53</v>
       </c>
@@ -1347,7 +1355,7 @@
       <c r="W11" s="3"/>
       <c r="X11" s="3"/>
     </row>
-    <row r="12" spans="1:24" ht="12.75">
+    <row r="12" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>29</v>
       </c>
@@ -1397,7 +1405,7 @@
       <c r="W12" s="3"/>
       <c r="X12" s="3"/>
     </row>
-    <row r="13" spans="1:24" ht="12.75">
+    <row r="13" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>61</v>
       </c>
@@ -1445,7 +1453,7 @@
       <c r="W13" s="3"/>
       <c r="X13" s="3"/>
     </row>
-    <row r="14" spans="1:24" ht="12.75">
+    <row r="14" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>64</v>
       </c>
@@ -1499,7 +1507,7 @@
       <c r="W14" s="3"/>
       <c r="X14" s="3"/>
     </row>
-    <row r="15" spans="1:24" ht="12.75">
+    <row r="15" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>66</v>
       </c>
@@ -1561,7 +1569,7 @@
       <c r="W15" s="3"/>
       <c r="X15" s="3"/>
     </row>
-    <row r="16" spans="1:24" s="3" customFormat="1" ht="12.75">
+    <row r="16" spans="1:24" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>71</v>
       </c>
@@ -1596,7 +1604,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:24" ht="12.75">
+    <row r="17" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>73</v>
       </c>
@@ -1652,7 +1660,7 @@
       <c r="W17" s="3"/>
       <c r="X17" s="3"/>
     </row>
-    <row r="18" spans="1:24" ht="15.75" customHeight="1">
+    <row r="18" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>50</v>
       </c>
@@ -1704,7 +1712,7 @@
       <c r="W18" s="3"/>
       <c r="X18" s="3"/>
     </row>
-    <row r="19" spans="1:24" ht="15.75" customHeight="1">
+    <row r="19" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>78</v>
       </c>
@@ -1758,7 +1766,7 @@
       <c r="W19" s="3"/>
       <c r="X19" s="3"/>
     </row>
-    <row r="20" spans="1:24" ht="15.75" customHeight="1">
+    <row r="20" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>81</v>
       </c>
@@ -1814,7 +1822,7 @@
       <c r="W20" s="3"/>
       <c r="X20" s="3"/>
     </row>
-    <row r="21" spans="1:24" ht="15.75" customHeight="1">
+    <row r="21" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>16</v>
       </c>
@@ -1858,7 +1866,7 @@
       <c r="W21" s="3"/>
       <c r="X21" s="3"/>
     </row>
-    <row r="22" spans="1:24" ht="15.75" customHeight="1">
+    <row r="22" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>17</v>
       </c>
@@ -1902,7 +1910,7 @@
       <c r="W22" s="3"/>
       <c r="X22" s="3"/>
     </row>
-    <row r="23" spans="1:24" ht="15.75" customHeight="1">
+    <row r="23" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>58</v>
       </c>
@@ -1936,7 +1944,7 @@
       <c r="W23" s="3"/>
       <c r="X23" s="3"/>
     </row>
-    <row r="24" spans="1:24" ht="15.75" customHeight="1">
+    <row r="24" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>18</v>
       </c>
@@ -1970,7 +1978,7 @@
       <c r="W24" s="3"/>
       <c r="X24" s="3"/>
     </row>
-    <row r="25" spans="1:24" ht="15.75" customHeight="1">
+    <row r="25" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>59</v>
       </c>
@@ -2004,7 +2012,7 @@
       <c r="W25" s="3"/>
       <c r="X25" s="3"/>
     </row>
-    <row r="26" spans="1:24" ht="15.75" customHeight="1">
+    <row r="26" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>84</v>
       </c>
@@ -2040,7 +2048,7 @@
       <c r="W26" s="3"/>
       <c r="X26" s="3"/>
     </row>
-    <row r="27" spans="1:24" ht="15.75" customHeight="1">
+    <row r="27" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>19</v>
       </c>
@@ -2076,7 +2084,7 @@
       <c r="W27" s="3"/>
       <c r="X27" s="3"/>
     </row>
-    <row r="28" spans="1:24" ht="15.75" customHeight="1">
+    <row r="28" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>51</v>
       </c>
@@ -2110,7 +2118,7 @@
       <c r="W28" s="3"/>
       <c r="X28" s="3"/>
     </row>
-    <row r="29" spans="1:24" ht="15.75" customHeight="1">
+    <row r="29" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>88</v>
       </c>
@@ -2146,9 +2154,9 @@
       <c r="W29" s="3"/>
       <c r="X29" s="3"/>
     </row>
-    <row r="30" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A30" s="5" t="s">
-        <v>13</v>
+    <row r="30" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -2159,24 +2167,33 @@
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
+      <c r="K30" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="N30" s="3"/>
-      <c r="O30" s="3"/>
-      <c r="P30" s="3"/>
-      <c r="Q30" s="3"/>
-      <c r="R30" s="3"/>
+      <c r="O30" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="P30" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q30" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R30" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="S30" s="3"/>
-      <c r="T30" s="3"/>
-      <c r="U30" s="3"/>
-      <c r="V30" s="3"/>
-      <c r="W30" s="3"/>
-      <c r="X30" s="3"/>
-    </row>
-    <row r="31" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A31" s="2" t="s">
-        <v>14</v>
+    </row>
+    <row r="31" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -2187,24 +2204,37 @@
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
-      <c r="N31" s="3"/>
-      <c r="O31" s="3"/>
-      <c r="P31" s="3"/>
-      <c r="Q31" s="3"/>
-      <c r="R31" s="3"/>
-      <c r="S31" s="3"/>
-      <c r="T31" s="3"/>
-      <c r="U31" s="3"/>
-      <c r="V31" s="3"/>
-      <c r="W31" s="3"/>
-      <c r="X31" s="3"/>
-    </row>
-    <row r="32" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A32" s="2" t="s">
-        <v>15</v>
+      <c r="K31" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="N31" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O31" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="P31" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q31" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="R31" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="S31" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>90</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -2215,74 +2245,129 @@
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
-      <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
+      <c r="K32" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="M32" s="3"/>
       <c r="N32" s="3"/>
-      <c r="O32" s="3"/>
-      <c r="P32" s="3"/>
-      <c r="Q32" s="3"/>
+      <c r="O32" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="P32" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q32" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="R32" s="3"/>
       <c r="S32" s="3"/>
-      <c r="T32" s="3"/>
-      <c r="U32" s="3"/>
-      <c r="V32" s="3"/>
-      <c r="W32" s="3"/>
-      <c r="X32" s="3"/>
-    </row>
-    <row r="33" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A33" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A34" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A35" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A36" s="2" t="s">
+    </row>
+    <row r="33" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M33" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="N33" s="3"/>
+      <c r="O33" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P33" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R33" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="S33" s="3"/>
+    </row>
+    <row r="34" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="L34" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A37" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A38" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A39" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A40" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A41" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A42" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A43" s="3" t="s">
-        <v>89</v>
+      <c r="M34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N34" s="3"/>
+      <c r="O34" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="P34" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q34" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="R34" s="3"/>
+      <c r="S34" s="3"/>
+    </row>
+    <row r="35" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="M35" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N35" s="3"/>
+      <c r="O35" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="P35" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q35" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -2292,14 +2377,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31648440-34B2-41E0-A4DA-8D4AD12FC756}">
-  <dimension ref="A1:AX43"/>
+  <dimension ref="A1:AV35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0" xr3:uid="{354EE10B-ACE1-5338-88D3-2FA0829946D8}">
-      <pane xSplit="2" topLeftCell="V1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="W37" sqref="W37"/>
+    <sheetView topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.85546875" style="6" bestFit="1" customWidth="1"/>
@@ -2323,21 +2408,21 @@
     <col min="20" max="20" width="5.7109375" style="6" customWidth="1"/>
     <col min="21" max="21" width="14.42578125" style="6"/>
     <col min="22" max="22" width="5.7109375" style="6" customWidth="1"/>
-    <col min="23" max="23" width="14.42578125" style="6"/>
-    <col min="24" max="24" width="5.7109375" style="6" customWidth="1"/>
-    <col min="25" max="25" width="18" style="7" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18" style="7" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.42578125" style="6"/>
     <col min="26" max="26" width="5.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.42578125" style="6"/>
-    <col min="28" max="28" width="5.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="15" style="6" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15" style="6" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="5.7109375" style="6" customWidth="1"/>
+    <col min="29" max="29" width="14.42578125" style="6"/>
     <col min="30" max="30" width="5.7109375" style="6" customWidth="1"/>
-    <col min="31" max="31" width="14.42578125" style="6"/>
+    <col min="31" max="31" width="18" style="6" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="5.7109375" style="6" customWidth="1"/>
-    <col min="33" max="33" width="18" style="6" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.42578125" style="6"/>
     <col min="34" max="34" width="5.7109375" style="6" customWidth="1"/>
-    <col min="35" max="35" width="14.42578125" style="6"/>
+    <col min="35" max="35" width="13.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="5.7109375" style="6" customWidth="1"/>
-    <col min="37" max="37" width="13.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="14.42578125" style="6"/>
     <col min="38" max="38" width="5.7109375" style="6" customWidth="1"/>
     <col min="39" max="39" width="14.42578125" style="6"/>
     <col min="40" max="40" width="5.7109375" style="6" customWidth="1"/>
@@ -2349,172 +2434,164 @@
     <col min="46" max="46" width="5.7109375" style="6" customWidth="1"/>
     <col min="47" max="47" width="14.42578125" style="6"/>
     <col min="48" max="48" width="5.7109375" style="6" customWidth="1"/>
-    <col min="49" max="49" width="14.42578125" style="6"/>
-    <col min="50" max="50" width="5.7109375" style="6" customWidth="1"/>
-    <col min="51" max="16384" width="14.42578125" style="6"/>
+    <col min="49" max="16384" width="14.42578125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" ht="12.75">
+    <row r="1" spans="1:48" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>4</v>
+        <v>96</v>
+      </c>
+      <c r="W1" s="8" t="s">
+        <v>5</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="Y1" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="AC1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="AE1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="AG1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="AI1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
+      </c>
+      <c r="AK1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="AL1" s="4" t="s">
+        <v>96</v>
       </c>
       <c r="AM1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="AN1" s="4" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="AO1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="AP1" s="4" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="AQ1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="AR1" s="4" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="AS1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="AT1" s="4" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="AU1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="AV1" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="AW1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="AX1" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:50" ht="12.75">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:48" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -2543,100 +2620,94 @@
       <c r="N2" s="6">
         <v>0.3</v>
       </c>
-      <c r="W2" s="2" t="s">
-        <v>12</v>
+      <c r="W2" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="X2" s="6">
-        <v>1</v>
-      </c>
-      <c r="Y2" s="7" t="s">
-        <v>13</v>
+        <v>0.8</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="Z2" s="6">
-        <v>0.8</v>
+        <v>0.87</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AB2" s="6">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD2" s="6">
+        <v>-1</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF2" s="6">
+        <v>-0.28999999999999998</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH2" s="6">
+        <v>-1</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ2" s="6">
+        <v>-0.79</v>
+      </c>
+      <c r="AK2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL2" s="6">
         <v>0.87</v>
       </c>
-      <c r="AC2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD2" s="6">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AF2" s="6">
-        <v>-1</v>
-      </c>
-      <c r="AG2" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH2" s="6">
-        <v>-0.28999999999999998</v>
-      </c>
-      <c r="AI2" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AJ2" s="6">
-        <v>-1</v>
-      </c>
-      <c r="AK2" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AL2" s="6">
-        <v>-0.79</v>
-      </c>
       <c r="AM2" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AN2" s="6">
         <v>0.87</v>
       </c>
       <c r="AO2" s="6" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="AP2" s="6">
-        <v>0.87</v>
+        <v>-0.59</v>
       </c>
       <c r="AQ2" s="6" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="AR2" s="6">
-        <v>-0.59</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AS2" s="6" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="AT2" s="6">
-        <v>0.55000000000000004</v>
+        <v>-0.79</v>
       </c>
       <c r="AU2" s="6" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="AV2" s="6">
-        <v>-0.79</v>
-      </c>
-      <c r="AW2" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="AX2" s="6">
         <v>-0.28999999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:50" s="10" customFormat="1" ht="12.75">
+    <row r="3" spans="1:48" s="10" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D3" s="9">
         <v>1</v>
@@ -2653,100 +2724,94 @@
       <c r="L3" s="10">
         <v>1</v>
       </c>
-      <c r="W3" s="9" t="s">
-        <v>23</v>
+      <c r="W3" s="11" t="s">
+        <v>13</v>
       </c>
       <c r="X3" s="10">
-        <v>1</v>
-      </c>
-      <c r="Y3" s="11" t="s">
-        <v>13</v>
+        <v>0.15</v>
+      </c>
+      <c r="Y3" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="Z3" s="10">
-        <v>0.15</v>
+        <v>0.71</v>
       </c>
       <c r="AA3" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AB3" s="10">
-        <v>0.71</v>
+        <v>0.74</v>
       </c>
       <c r="AC3" s="9" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="AD3" s="10">
-        <v>0.74</v>
+        <v>-1</v>
       </c>
       <c r="AE3" s="9" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="AF3" s="10">
+        <v>-0.48</v>
+      </c>
+      <c r="AG3" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH3" s="10">
         <v>-1</v>
       </c>
-      <c r="AG3" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH3" s="10">
-        <v>-0.48</v>
-      </c>
       <c r="AI3" s="9" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="AJ3" s="10">
-        <v>-1</v>
-      </c>
-      <c r="AK3" s="9" t="s">
-        <v>57</v>
+        <v>-0.74</v>
+      </c>
+      <c r="AK3" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="AL3" s="10">
-        <v>-0.74</v>
+        <v>0.91</v>
       </c>
       <c r="AM3" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AN3" s="10">
         <v>0.91</v>
       </c>
       <c r="AO3" s="10" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="AP3" s="10">
-        <v>0.91</v>
+        <v>-0.54</v>
       </c>
       <c r="AQ3" s="10" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="AR3" s="10">
-        <v>-0.54</v>
+        <v>0.74</v>
       </c>
       <c r="AS3" s="10" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="AT3" s="10">
-        <v>0.74</v>
+        <v>-0.74</v>
       </c>
       <c r="AU3" s="10" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="AV3" s="10">
-        <v>-0.74</v>
-      </c>
-      <c r="AW3" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="AX3" s="10">
         <v>-0.48</v>
       </c>
     </row>
-    <row r="4" spans="1:50" ht="12.75">
+    <row r="4" spans="1:48" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
@@ -2787,97 +2852,91 @@
       <c r="T4" s="6">
         <v>0.3</v>
       </c>
-      <c r="W4" s="2" t="s">
-        <v>23</v>
+      <c r="W4" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="X4" s="6">
-        <v>1</v>
-      </c>
-      <c r="Y4" s="7" t="s">
-        <v>13</v>
+        <v>0.71</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="Z4" s="6">
-        <v>0.71</v>
+        <v>0.78</v>
       </c>
       <c r="AA4" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AB4" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AC4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD4" s="6">
+        <v>-1</v>
+      </c>
+      <c r="AE4" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF4" s="6">
+        <v>-0.5</v>
+      </c>
+      <c r="AG4" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH4" s="6">
+        <v>-1</v>
+      </c>
+      <c r="AI4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ4" s="6">
+        <v>-0.75</v>
+      </c>
+      <c r="AK4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL4" s="6">
         <v>0.78</v>
       </c>
-      <c r="AC4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD4" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="AE4" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AF4" s="6">
-        <v>-1</v>
-      </c>
-      <c r="AG4" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH4" s="6">
-        <v>-0.5</v>
-      </c>
-      <c r="AI4" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AJ4" s="6">
-        <v>-1</v>
-      </c>
-      <c r="AK4" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AL4" s="6">
-        <v>-0.75</v>
-      </c>
       <c r="AM4" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AN4" s="6">
         <v>0.78</v>
       </c>
       <c r="AO4" s="6" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="AP4" s="6">
-        <v>0.78</v>
+        <v>-0.65</v>
       </c>
       <c r="AQ4" s="6" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="AR4" s="6">
-        <v>-0.65</v>
+        <v>0.5</v>
       </c>
       <c r="AS4" s="6" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="AT4" s="6">
-        <v>0.5</v>
+        <v>-0.75</v>
       </c>
       <c r="AU4" s="6" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="AV4" s="6">
-        <v>-0.75</v>
-      </c>
-      <c r="AW4" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="AX4" s="6">
         <v>-0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:50" ht="12.75">
+    <row r="5" spans="1:48" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
@@ -2898,97 +2957,91 @@
       <c r="R5" s="6">
         <v>1</v>
       </c>
-      <c r="W5" s="2" t="s">
-        <v>33</v>
+      <c r="W5" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="X5" s="6">
-        <v>1</v>
-      </c>
-      <c r="Y5" s="7" t="s">
-        <v>13</v>
+        <v>0.35</v>
+      </c>
+      <c r="Y5" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="Z5" s="6">
-        <v>0.35</v>
+        <v>0.78</v>
       </c>
       <c r="AA5" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AB5" s="6">
+        <v>0.51</v>
+      </c>
+      <c r="AC5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD5" s="6">
+        <v>-1</v>
+      </c>
+      <c r="AE5" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF5" s="6">
+        <v>-0.49</v>
+      </c>
+      <c r="AG5" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH5" s="6">
+        <v>-1</v>
+      </c>
+      <c r="AI5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ5" s="6">
+        <v>-0.65</v>
+      </c>
+      <c r="AK5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL5" s="6">
         <v>0.78</v>
       </c>
-      <c r="AC5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD5" s="6">
-        <v>0.51</v>
-      </c>
-      <c r="AE5" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AF5" s="6">
-        <v>-1</v>
-      </c>
-      <c r="AG5" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH5" s="6">
-        <v>-0.49</v>
-      </c>
-      <c r="AI5" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AJ5" s="6">
-        <v>-1</v>
-      </c>
-      <c r="AK5" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AL5" s="6">
-        <v>-0.65</v>
-      </c>
       <c r="AM5" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AN5" s="6">
         <v>0.78</v>
       </c>
       <c r="AO5" s="6" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="AP5" s="6">
-        <v>0.78</v>
+        <v>-0.55000000000000004</v>
       </c>
       <c r="AQ5" s="6" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="AR5" s="6">
-        <v>-0.55000000000000004</v>
+        <v>0.51</v>
       </c>
       <c r="AS5" s="6" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="AT5" s="6">
-        <v>0.51</v>
+        <v>-0.65</v>
       </c>
       <c r="AU5" s="6" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="AV5" s="6">
-        <v>-0.65</v>
-      </c>
-      <c r="AW5" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="AX5" s="6">
         <v>-0.49</v>
       </c>
     </row>
-    <row r="6" spans="1:50" ht="12.75">
+    <row r="6" spans="1:48" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
@@ -3009,92 +3062,86 @@
       <c r="R6" s="6">
         <v>1</v>
       </c>
-      <c r="W6" s="2" t="s">
-        <v>33</v>
+      <c r="W6" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="X6" s="6">
-        <v>1</v>
-      </c>
-      <c r="Y6" s="7" t="s">
-        <v>13</v>
+        <v>0.35</v>
+      </c>
+      <c r="Y6" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="Z6" s="6">
-        <v>0.35</v>
+        <v>0.62</v>
       </c>
       <c r="AA6" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AB6" s="6">
+        <v>0.47</v>
+      </c>
+      <c r="AC6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD6" s="6">
+        <v>-1</v>
+      </c>
+      <c r="AE6" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF6" s="6">
+        <v>-0.47</v>
+      </c>
+      <c r="AG6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH6" s="6">
+        <v>-1</v>
+      </c>
+      <c r="AI6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ6" s="6">
+        <v>-0.35</v>
+      </c>
+      <c r="AK6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL6" s="6">
         <v>0.62</v>
       </c>
-      <c r="AC6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD6" s="6">
-        <v>0.47</v>
-      </c>
-      <c r="AE6" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AF6" s="6">
-        <v>-1</v>
-      </c>
-      <c r="AG6" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH6" s="6">
-        <v>-0.47</v>
-      </c>
-      <c r="AI6" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AJ6" s="6">
-        <v>-1</v>
-      </c>
-      <c r="AK6" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AL6" s="6">
-        <v>-0.35</v>
-      </c>
       <c r="AM6" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AN6" s="6">
         <v>0.62</v>
       </c>
       <c r="AO6" s="6" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="AP6" s="6">
-        <v>0.62</v>
+        <v>-0.33</v>
       </c>
       <c r="AQ6" s="6" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="AR6" s="6">
-        <v>-0.33</v>
+        <v>0.47</v>
       </c>
       <c r="AS6" s="6" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="AT6" s="6">
-        <v>0.47</v>
+        <v>-0.35</v>
       </c>
       <c r="AU6" s="6" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="AV6" s="6">
-        <v>-0.35</v>
-      </c>
-      <c r="AW6" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="AX6" s="6">
         <v>-0.47</v>
       </c>
     </row>
-    <row r="7" spans="1:50" ht="12.75">
+    <row r="7" spans="1:48" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>37</v>
       </c>
@@ -3114,100 +3161,94 @@
       <c r="L7" s="6">
         <v>1</v>
       </c>
-      <c r="W7" s="2" t="s">
-        <v>23</v>
+      <c r="W7" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="X7" s="6">
-        <v>1</v>
-      </c>
-      <c r="Y7" s="7" t="s">
-        <v>13</v>
+        <v>0.5</v>
+      </c>
+      <c r="Y7" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="Z7" s="6">
-        <v>0.5</v>
+        <v>0.65</v>
       </c>
       <c r="AA7" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AB7" s="6">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="AC7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD7" s="6">
+        <v>-1</v>
+      </c>
+      <c r="AE7" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF7" s="6">
+        <v>-0.55000000000000004</v>
+      </c>
+      <c r="AG7" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH7" s="6">
+        <v>-1</v>
+      </c>
+      <c r="AI7" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ7" s="6">
+        <v>-0.4</v>
+      </c>
+      <c r="AK7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL7" s="6">
         <v>0.65</v>
       </c>
-      <c r="AC7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD7" s="6">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="AE7" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AF7" s="6">
-        <v>-1</v>
-      </c>
-      <c r="AG7" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH7" s="6">
-        <v>-0.55000000000000004</v>
-      </c>
-      <c r="AI7" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AJ7" s="6">
-        <v>-1</v>
-      </c>
-      <c r="AK7" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AL7" s="6">
-        <v>-0.4</v>
-      </c>
       <c r="AM7" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AN7" s="6">
         <v>0.65</v>
       </c>
       <c r="AO7" s="6" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="AP7" s="6">
-        <v>0.65</v>
+        <v>-0.3</v>
       </c>
       <c r="AQ7" s="6" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="AR7" s="6">
-        <v>-0.3</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AS7" s="6" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="AT7" s="6">
-        <v>0.55000000000000004</v>
+        <v>-0.4</v>
       </c>
       <c r="AU7" s="6" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="AV7" s="6">
-        <v>-0.4</v>
-      </c>
-      <c r="AW7" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="AX7" s="6">
         <v>-0.55000000000000004</v>
       </c>
     </row>
-    <row r="8" spans="1:50" ht="12.75">
+    <row r="8" spans="1:48" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D8" s="2">
         <v>1</v>
@@ -3254,97 +3295,91 @@
       <c r="R8" s="6">
         <v>1</v>
       </c>
-      <c r="W8" s="2" t="s">
-        <v>33</v>
+      <c r="W8" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="X8" s="6">
-        <v>1</v>
-      </c>
-      <c r="Y8" s="7" t="s">
-        <v>13</v>
+        <v>0.62</v>
+      </c>
+      <c r="Y8" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="Z8" s="6">
-        <v>0.62</v>
+        <v>0.75</v>
       </c>
       <c r="AA8" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AB8" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AC8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD8" s="6">
+        <v>-1</v>
+      </c>
+      <c r="AE8" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF8" s="6">
+        <v>-0.2</v>
+      </c>
+      <c r="AG8" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH8" s="6">
+        <v>-1</v>
+      </c>
+      <c r="AI8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ8" s="6">
+        <v>-0.49</v>
+      </c>
+      <c r="AK8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL8" s="6">
         <v>0.75</v>
       </c>
-      <c r="AC8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD8" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="AE8" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AF8" s="6">
-        <v>-1</v>
-      </c>
-      <c r="AG8" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH8" s="6">
-        <v>-0.2</v>
-      </c>
-      <c r="AI8" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AJ8" s="6">
-        <v>-1</v>
-      </c>
-      <c r="AK8" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AL8" s="6">
-        <v>-0.49</v>
-      </c>
       <c r="AM8" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AN8" s="6">
         <v>0.75</v>
       </c>
       <c r="AO8" s="6" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="AP8" s="6">
-        <v>0.75</v>
+        <v>-0.39</v>
       </c>
       <c r="AQ8" s="6" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="AR8" s="6">
-        <v>-0.39</v>
+        <v>0.5</v>
       </c>
       <c r="AS8" s="6" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="AT8" s="6">
-        <v>0.5</v>
+        <v>-0.49</v>
       </c>
       <c r="AU8" s="6" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="AV8" s="6">
-        <v>-0.49</v>
-      </c>
-      <c r="AW8" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="AX8" s="6">
         <v>-0.2</v>
       </c>
     </row>
-    <row r="9" spans="1:50" ht="12.75">
+    <row r="9" spans="1:48" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>46</v>
@@ -3382,97 +3417,91 @@
       <c r="T9" s="6">
         <v>0.2</v>
       </c>
-      <c r="W9" s="2" t="s">
-        <v>33</v>
+      <c r="W9" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="X9" s="6">
-        <v>1</v>
-      </c>
-      <c r="Y9" s="7" t="s">
-        <v>13</v>
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="Y9" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="Z9" s="6">
-        <v>0.57999999999999996</v>
+        <v>0.8</v>
       </c>
       <c r="AA9" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AB9" s="6">
+        <v>0.79</v>
+      </c>
+      <c r="AC9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD9" s="6">
+        <v>-1</v>
+      </c>
+      <c r="AE9" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF9" s="6">
+        <v>-0.6</v>
+      </c>
+      <c r="AG9" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH9" s="6">
+        <v>-0.35</v>
+      </c>
+      <c r="AI9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ9" s="6">
+        <v>-0.47</v>
+      </c>
+      <c r="AK9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL9" s="6">
         <v>0.8</v>
       </c>
-      <c r="AC9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD9" s="6">
-        <v>0.79</v>
-      </c>
-      <c r="AE9" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AF9" s="6">
-        <v>-1</v>
-      </c>
-      <c r="AG9" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH9" s="6">
-        <v>-0.6</v>
-      </c>
-      <c r="AI9" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AJ9" s="6">
-        <v>-0.35</v>
-      </c>
-      <c r="AK9" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AL9" s="6">
-        <v>-0.47</v>
-      </c>
       <c r="AM9" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AN9" s="6">
         <v>0.8</v>
       </c>
       <c r="AO9" s="6" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="AP9" s="6">
-        <v>0.8</v>
+        <v>-0.37</v>
       </c>
       <c r="AQ9" s="6" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="AR9" s="6">
-        <v>-0.37</v>
+        <v>0.79</v>
       </c>
       <c r="AS9" s="6" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="AT9" s="6">
-        <v>0.79</v>
+        <v>-0.47</v>
       </c>
       <c r="AU9" s="6" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="AV9" s="6">
-        <v>-0.47</v>
-      </c>
-      <c r="AW9" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="AX9" s="6">
         <v>-0.6</v>
       </c>
     </row>
-    <row r="10" spans="1:50" ht="12.75">
+    <row r="10" spans="1:48" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>52</v>
@@ -3504,97 +3533,91 @@
       <c r="R10" s="6">
         <v>1</v>
       </c>
-      <c r="W10" s="2" t="s">
-        <v>33</v>
+      <c r="W10" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="X10" s="6">
-        <v>1</v>
-      </c>
-      <c r="Y10" s="7" t="s">
-        <v>13</v>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="Y10" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="Z10" s="6">
-        <v>0.28000000000000003</v>
+        <v>0.81</v>
       </c>
       <c r="AA10" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AB10" s="6">
+        <v>0.88</v>
+      </c>
+      <c r="AC10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD10" s="6">
+        <v>-1</v>
+      </c>
+      <c r="AE10" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF10" s="6">
+        <v>-0.74</v>
+      </c>
+      <c r="AG10" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH10" s="6">
+        <v>0.42</v>
+      </c>
+      <c r="AI10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ10" s="6">
+        <v>-0.55000000000000004</v>
+      </c>
+      <c r="AK10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL10" s="6">
         <v>0.81</v>
       </c>
-      <c r="AC10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD10" s="6">
-        <v>0.88</v>
-      </c>
-      <c r="AE10" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AF10" s="6">
-        <v>-1</v>
-      </c>
-      <c r="AG10" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH10" s="6">
-        <v>-0.74</v>
-      </c>
-      <c r="AI10" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AJ10" s="6">
-        <v>0.42</v>
-      </c>
-      <c r="AK10" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AL10" s="6">
-        <v>-0.55000000000000004</v>
-      </c>
       <c r="AM10" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AN10" s="6">
         <v>0.81</v>
       </c>
       <c r="AO10" s="6" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="AP10" s="6">
-        <v>0.81</v>
+        <v>-0.45</v>
       </c>
       <c r="AQ10" s="6" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="AR10" s="6">
-        <v>-0.45</v>
+        <v>0.88</v>
       </c>
       <c r="AS10" s="6" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="AT10" s="6">
-        <v>0.88</v>
+        <v>-0.55000000000000004</v>
       </c>
       <c r="AU10" s="6" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="AV10" s="6">
-        <v>-0.55000000000000004</v>
-      </c>
-      <c r="AW10" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="AX10" s="6">
         <v>-0.74</v>
       </c>
     </row>
-    <row r="11" spans="1:50" ht="12.75">
+    <row r="11" spans="1:48" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>21</v>
@@ -3608,100 +3631,94 @@
       <c r="L11" s="6">
         <v>1</v>
       </c>
-      <c r="W11" s="2" t="s">
-        <v>55</v>
+      <c r="W11" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="X11" s="6">
+        <v>-0.88</v>
+      </c>
+      <c r="Y11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z11" s="6">
+        <v>-0.9</v>
+      </c>
+      <c r="AA11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB11" s="6">
+        <v>-0.95</v>
+      </c>
+      <c r="AC11" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD11" s="6">
         <v>1</v>
       </c>
-      <c r="Y11" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z11" s="6">
-        <v>-0.88</v>
-      </c>
-      <c r="AA11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB11" s="6">
+      <c r="AE11" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF11" s="6">
+        <v>-0.75</v>
+      </c>
+      <c r="AG11" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH11" s="6">
+        <v>-1</v>
+      </c>
+      <c r="AI11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ11" s="6">
+        <v>1</v>
+      </c>
+      <c r="AK11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL11" s="6">
         <v>-0.9</v>
       </c>
-      <c r="AC11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD11" s="6">
-        <v>-0.95</v>
-      </c>
-      <c r="AE11" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AF11" s="6">
-        <v>1</v>
-      </c>
-      <c r="AG11" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH11" s="6">
-        <v>-0.75</v>
-      </c>
-      <c r="AI11" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AJ11" s="6">
-        <v>-1</v>
-      </c>
-      <c r="AK11" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AL11" s="6">
-        <v>1</v>
-      </c>
       <c r="AM11" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AN11" s="6">
         <v>-0.9</v>
       </c>
       <c r="AO11" s="6" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="AP11" s="6">
-        <v>-0.9</v>
+        <v>0.89</v>
       </c>
       <c r="AQ11" s="6" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="AR11" s="6">
-        <v>0.89</v>
+        <v>-0.95</v>
       </c>
       <c r="AS11" s="6" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="AT11" s="6">
-        <v>-0.95</v>
+        <v>1</v>
       </c>
       <c r="AU11" s="6" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="AV11" s="6">
-        <v>1</v>
-      </c>
-      <c r="AW11" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="AX11" s="6">
         <v>-0.75</v>
       </c>
     </row>
-    <row r="12" spans="1:50" ht="12.75">
+    <row r="12" spans="1:48" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>29</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D12" s="6">
         <v>1</v>
@@ -3724,100 +3741,94 @@
       <c r="R12" s="6">
         <v>1</v>
       </c>
-      <c r="W12" s="2" t="s">
-        <v>23</v>
+      <c r="W12" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="X12" s="6">
-        <v>1</v>
-      </c>
-      <c r="Y12" s="7" t="s">
-        <v>13</v>
+        <v>0.75</v>
+      </c>
+      <c r="Y12" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="Z12" s="6">
-        <v>0.75</v>
+        <v>0.74</v>
       </c>
       <c r="AA12" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AB12" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="AC12" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD12" s="6">
+        <v>-1</v>
+      </c>
+      <c r="AE12" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF12" s="6">
+        <v>-0.6</v>
+      </c>
+      <c r="AG12" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH12" s="6">
+        <v>-1</v>
+      </c>
+      <c r="AI12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ12" s="6">
+        <v>-0.26</v>
+      </c>
+      <c r="AK12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL12" s="6">
         <v>0.74</v>
       </c>
-      <c r="AC12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD12" s="6">
-        <v>0.7</v>
-      </c>
-      <c r="AE12" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AF12" s="6">
-        <v>-1</v>
-      </c>
-      <c r="AG12" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH12" s="6">
-        <v>-0.6</v>
-      </c>
-      <c r="AI12" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AJ12" s="6">
-        <v>-1</v>
-      </c>
-      <c r="AK12" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AL12" s="6">
-        <v>-0.26</v>
-      </c>
       <c r="AM12" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AN12" s="6">
         <v>0.74</v>
       </c>
       <c r="AO12" s="6" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="AP12" s="6">
-        <v>0.74</v>
+        <v>-0.16</v>
       </c>
       <c r="AQ12" s="6" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="AR12" s="6">
-        <v>-0.16</v>
+        <v>0.7</v>
       </c>
       <c r="AS12" s="6" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="AT12" s="6">
-        <v>0.7</v>
+        <v>-0.26</v>
       </c>
       <c r="AU12" s="6" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="AV12" s="6">
-        <v>-0.26</v>
-      </c>
-      <c r="AW12" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="AX12" s="6">
         <v>-0.6</v>
       </c>
     </row>
-    <row r="13" spans="1:50" ht="12.75">
+    <row r="13" spans="1:48" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D13" s="6">
         <v>1</v>
@@ -3834,97 +3845,91 @@
       <c r="L13" s="6">
         <v>1</v>
       </c>
-      <c r="W13" s="2" t="s">
-        <v>33</v>
+      <c r="W13" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="X13" s="6">
-        <v>1</v>
-      </c>
-      <c r="Y13" s="7" t="s">
-        <v>13</v>
+        <v>0.6</v>
+      </c>
+      <c r="Y13" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="Z13" s="6">
-        <v>0.6</v>
+        <v>0.73</v>
       </c>
       <c r="AA13" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AB13" s="6">
+        <v>0.51</v>
+      </c>
+      <c r="AC13" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD13" s="6">
+        <v>-1</v>
+      </c>
+      <c r="AE13" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF13" s="6">
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="AG13" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH13" s="6">
+        <v>-1</v>
+      </c>
+      <c r="AI13" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ13" s="6">
+        <v>-0.48</v>
+      </c>
+      <c r="AK13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL13" s="6">
         <v>0.73</v>
       </c>
-      <c r="AC13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD13" s="6">
-        <v>0.51</v>
-      </c>
-      <c r="AE13" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AF13" s="6">
-        <v>-1</v>
-      </c>
-      <c r="AG13" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH13" s="6">
-        <v>-0.14000000000000001</v>
-      </c>
-      <c r="AI13" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AJ13" s="6">
-        <v>-1</v>
-      </c>
-      <c r="AK13" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AL13" s="6">
-        <v>-0.48</v>
-      </c>
       <c r="AM13" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AN13" s="6">
         <v>0.73</v>
       </c>
       <c r="AO13" s="6" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="AP13" s="6">
-        <v>0.73</v>
+        <v>-0.38</v>
       </c>
       <c r="AQ13" s="6" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="AR13" s="6">
-        <v>-0.38</v>
+        <v>0.51</v>
       </c>
       <c r="AS13" s="6" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="AT13" s="6">
-        <v>0.51</v>
+        <v>-0.48</v>
       </c>
       <c r="AU13" s="6" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="AV13" s="6">
-        <v>-0.48</v>
-      </c>
-      <c r="AW13" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="AX13" s="6">
         <v>-0.14000000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:50" ht="12.75">
+    <row r="14" spans="1:48" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>38</v>
@@ -3956,97 +3961,91 @@
       <c r="R14" s="6">
         <v>1</v>
       </c>
-      <c r="W14" s="2" t="s">
-        <v>23</v>
+      <c r="W14" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="X14" s="6">
-        <v>1</v>
-      </c>
-      <c r="Y14" s="7" t="s">
-        <v>13</v>
+        <v>0.77</v>
+      </c>
+      <c r="Y14" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="Z14" s="6">
-        <v>0.77</v>
+        <v>0.86</v>
       </c>
       <c r="AA14" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AB14" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="AC14" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD14" s="6">
+        <v>-1</v>
+      </c>
+      <c r="AE14" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF14" s="6">
+        <v>-0.35</v>
+      </c>
+      <c r="AG14" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH14" s="6">
+        <v>-1</v>
+      </c>
+      <c r="AI14" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ14" s="6">
+        <v>-0.4</v>
+      </c>
+      <c r="AK14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL14" s="6">
         <v>0.86</v>
       </c>
-      <c r="AC14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD14" s="6">
-        <v>0.6</v>
-      </c>
-      <c r="AE14" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AF14" s="6">
-        <v>-1</v>
-      </c>
-      <c r="AG14" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH14" s="6">
-        <v>-0.35</v>
-      </c>
-      <c r="AI14" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AJ14" s="6">
-        <v>-1</v>
-      </c>
-      <c r="AK14" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AL14" s="6">
-        <v>-0.4</v>
-      </c>
       <c r="AM14" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AN14" s="6">
         <v>0.86</v>
       </c>
       <c r="AO14" s="6" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="AP14" s="6">
-        <v>0.86</v>
+        <v>-0.35</v>
       </c>
       <c r="AQ14" s="6" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="AR14" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="AS14" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="AT14" s="6">
+        <v>-0.4</v>
+      </c>
+      <c r="AU14" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="AV14" s="6">
         <v>-0.35</v>
       </c>
-      <c r="AS14" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="AT14" s="6">
-        <v>0.6</v>
-      </c>
-      <c r="AU14" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="AV14" s="6">
-        <v>-0.4</v>
-      </c>
-      <c r="AW14" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="AX14" s="6">
-        <v>-0.35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:50" ht="12.75">
+    </row>
+    <row r="15" spans="1:48" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>66</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>46</v>
@@ -4102,97 +4101,91 @@
       <c r="V15" s="6">
         <v>0.15</v>
       </c>
-      <c r="W15" s="2" t="s">
-        <v>55</v>
+      <c r="W15" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="X15" s="6">
-        <v>1</v>
-      </c>
-      <c r="Y15" s="7" t="s">
-        <v>13</v>
+        <v>-0.65</v>
+      </c>
+      <c r="Y15" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="Z15" s="6">
-        <v>-0.65</v>
+        <v>-0.32</v>
       </c>
       <c r="AA15" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AB15" s="6">
+        <v>0.86</v>
+      </c>
+      <c r="AC15" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD15" s="6">
+        <v>-1</v>
+      </c>
+      <c r="AE15" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF15" s="6">
+        <v>-0.05</v>
+      </c>
+      <c r="AG15" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH15" s="6">
+        <v>-1</v>
+      </c>
+      <c r="AI15" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ15" s="6">
+        <v>0.85</v>
+      </c>
+      <c r="AK15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL15" s="6">
         <v>-0.32</v>
       </c>
-      <c r="AC15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD15" s="6">
-        <v>0.86</v>
-      </c>
-      <c r="AE15" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AF15" s="6">
-        <v>-1</v>
-      </c>
-      <c r="AG15" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH15" s="6">
-        <v>-0.05</v>
-      </c>
-      <c r="AI15" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AJ15" s="6">
-        <v>-1</v>
-      </c>
-      <c r="AK15" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AL15" s="6">
-        <v>0.85</v>
-      </c>
       <c r="AM15" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AN15" s="6">
         <v>-0.32</v>
       </c>
       <c r="AO15" s="6" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="AP15" s="6">
-        <v>-0.32</v>
+        <v>0.75</v>
       </c>
       <c r="AQ15" s="6" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="AR15" s="6">
-        <v>0.75</v>
+        <v>0.86</v>
       </c>
       <c r="AS15" s="6" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="AT15" s="6">
-        <v>0.86</v>
+        <v>0.85</v>
       </c>
       <c r="AU15" s="6" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="AV15" s="6">
-        <v>0.85</v>
-      </c>
-      <c r="AW15" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="AX15" s="6">
         <v>-0.05</v>
       </c>
     </row>
-    <row r="16" spans="1:50" ht="12.75">
+    <row r="16" spans="1:48" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>72</v>
@@ -4218,97 +4211,91 @@
       <c r="N16" s="6">
         <v>0.15</v>
       </c>
-      <c r="W16" s="2" t="s">
-        <v>55</v>
+      <c r="W16" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="X16" s="6">
-        <v>1</v>
-      </c>
-      <c r="Y16" s="7" t="s">
-        <v>13</v>
+        <v>-0.65</v>
+      </c>
+      <c r="Y16" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="Z16" s="6">
-        <v>-0.65</v>
+        <v>-0.42</v>
       </c>
       <c r="AA16" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AB16" s="6">
+        <v>0.85</v>
+      </c>
+      <c r="AC16" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD16" s="6">
+        <v>-1</v>
+      </c>
+      <c r="AE16" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF16" s="6">
+        <v>-0.02</v>
+      </c>
+      <c r="AG16" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH16" s="6">
+        <v>-1</v>
+      </c>
+      <c r="AI16" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ16" s="6">
+        <v>0.85</v>
+      </c>
+      <c r="AK16" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL16" s="6">
         <v>-0.42</v>
       </c>
-      <c r="AC16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD16" s="6">
-        <v>0.85</v>
-      </c>
-      <c r="AE16" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AF16" s="6">
-        <v>-1</v>
-      </c>
-      <c r="AG16" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH16" s="6">
-        <v>-0.02</v>
-      </c>
-      <c r="AI16" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AJ16" s="6">
-        <v>-1</v>
-      </c>
-      <c r="AK16" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AL16" s="6">
-        <v>0.85</v>
-      </c>
       <c r="AM16" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AN16" s="6">
         <v>-0.42</v>
       </c>
       <c r="AO16" s="6" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="AP16" s="6">
-        <v>-0.42</v>
+        <v>0.75</v>
       </c>
       <c r="AQ16" s="6" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="AR16" s="6">
-        <v>0.75</v>
+        <v>0.85</v>
       </c>
       <c r="AS16" s="6" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="AT16" s="6">
         <v>0.85</v>
       </c>
       <c r="AU16" s="6" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="AV16" s="6">
-        <v>0.85</v>
-      </c>
-      <c r="AW16" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="AX16" s="6">
         <v>-0.02</v>
       </c>
     </row>
-    <row r="17" spans="1:50" ht="12.75">
+    <row r="17" spans="1:48" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>46</v>
@@ -4352,97 +4339,91 @@
       <c r="R17" s="6">
         <v>1</v>
       </c>
-      <c r="W17" s="2" t="s">
-        <v>55</v>
+      <c r="W17" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="X17" s="6">
-        <v>1</v>
-      </c>
-      <c r="Y17" s="7" t="s">
-        <v>13</v>
+        <v>-0.35</v>
+      </c>
+      <c r="Y17" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="Z17" s="6">
-        <v>-0.35</v>
+        <v>0.2</v>
       </c>
       <c r="AA17" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AB17" s="6">
+        <v>0.85</v>
+      </c>
+      <c r="AC17" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD17" s="6">
+        <v>-1</v>
+      </c>
+      <c r="AE17" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF17" s="6">
+        <v>-0.1</v>
+      </c>
+      <c r="AG17" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH17" s="6">
+        <v>-1</v>
+      </c>
+      <c r="AI17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ17" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="AK17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL17" s="6">
         <v>0.2</v>
       </c>
-      <c r="AC17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD17" s="6">
-        <v>0.85</v>
-      </c>
-      <c r="AE17" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AF17" s="6">
-        <v>-1</v>
-      </c>
-      <c r="AG17" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH17" s="6">
-        <v>-0.1</v>
-      </c>
-      <c r="AI17" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AJ17" s="6">
-        <v>-1</v>
-      </c>
-      <c r="AK17" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AL17" s="6">
-        <v>0.7</v>
-      </c>
       <c r="AM17" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AN17" s="6">
         <v>0.2</v>
       </c>
       <c r="AO17" s="6" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="AP17" s="6">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
       <c r="AQ17" s="6" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="AR17" s="6">
-        <v>0.6</v>
+        <v>0.85</v>
       </c>
       <c r="AS17" s="6" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="AT17" s="6">
-        <v>0.85</v>
+        <v>0.7</v>
       </c>
       <c r="AU17" s="6" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="AV17" s="6">
-        <v>0.7</v>
-      </c>
-      <c r="AW17" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="AX17" s="6">
         <v>-0.1</v>
       </c>
     </row>
-    <row r="18" spans="1:50" ht="15.75" customHeight="1">
+    <row r="18" spans="1:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>50</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>38</v>
@@ -4468,97 +4449,91 @@
       <c r="N18" s="6">
         <v>0.2</v>
       </c>
-      <c r="W18" s="6" t="s">
-        <v>33</v>
+      <c r="W18" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="X18" s="6">
-        <v>1</v>
-      </c>
-      <c r="Y18" s="7" t="s">
-        <v>13</v>
+        <v>0.35</v>
+      </c>
+      <c r="Y18" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="Z18" s="6">
-        <v>0.35</v>
+        <v>0.02</v>
       </c>
       <c r="AA18" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AB18" s="6">
+        <v>0.89</v>
+      </c>
+      <c r="AC18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD18" s="6">
+        <v>-1</v>
+      </c>
+      <c r="AE18" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF18" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="AG18" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH18" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="AI18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ18" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="AK18" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL18" s="6">
         <v>0.02</v>
       </c>
-      <c r="AC18" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD18" s="6">
-        <v>0.89</v>
-      </c>
-      <c r="AE18" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AF18" s="6">
-        <v>-1</v>
-      </c>
-      <c r="AG18" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH18" s="6">
-        <v>0.05</v>
-      </c>
-      <c r="AI18" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AJ18" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="AK18" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AL18" s="6">
-        <v>0.75</v>
-      </c>
       <c r="AM18" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AN18" s="6">
         <v>0.02</v>
       </c>
       <c r="AO18" s="6" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="AP18" s="6">
-        <v>0.02</v>
+        <v>0.65</v>
       </c>
       <c r="AQ18" s="6" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="AR18" s="6">
-        <v>0.65</v>
+        <v>0.89</v>
       </c>
       <c r="AS18" s="6" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="AT18" s="6">
-        <v>0.89</v>
+        <v>0.75</v>
       </c>
       <c r="AU18" s="6" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="AV18" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AW18" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="AX18" s="6">
         <v>0.05</v>
       </c>
     </row>
-    <row r="19" spans="1:50" ht="15.75" customHeight="1">
+    <row r="19" spans="1:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>78</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>52</v>
@@ -4590,97 +4565,91 @@
       <c r="R19" s="6">
         <v>1</v>
       </c>
-      <c r="W19" s="6" t="s">
-        <v>23</v>
+      <c r="W19" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="X19" s="6">
-        <v>1</v>
-      </c>
-      <c r="Y19" s="7" t="s">
-        <v>13</v>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Y19" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="Z19" s="6">
-        <v>7.0000000000000007E-2</v>
+        <v>-0.45</v>
       </c>
       <c r="AA19" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AB19" s="6">
+        <v>0.32</v>
+      </c>
+      <c r="AC19" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD19" s="6">
+        <v>-1</v>
+      </c>
+      <c r="AE19" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF19" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="AG19" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH19" s="6">
+        <v>0.65</v>
+      </c>
+      <c r="AI19" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ19" s="6">
+        <v>0.64</v>
+      </c>
+      <c r="AK19" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL19" s="6">
         <v>-0.45</v>
       </c>
-      <c r="AC19" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD19" s="6">
-        <v>0.32</v>
-      </c>
-      <c r="AE19" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AF19" s="6">
-        <v>-1</v>
-      </c>
-      <c r="AG19" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH19" s="6">
-        <v>0.9</v>
-      </c>
-      <c r="AI19" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AJ19" s="6">
-        <v>0.65</v>
-      </c>
-      <c r="AK19" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AL19" s="6">
-        <v>0.64</v>
-      </c>
       <c r="AM19" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AN19" s="6">
         <v>-0.45</v>
       </c>
       <c r="AO19" s="6" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="AP19" s="6">
-        <v>-0.45</v>
+        <v>0.54</v>
       </c>
       <c r="AQ19" s="6" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="AR19" s="6">
-        <v>0.54</v>
+        <v>0.32</v>
       </c>
       <c r="AS19" s="6" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="AT19" s="6">
-        <v>0.32</v>
+        <v>0.64</v>
       </c>
       <c r="AU19" s="6" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="AV19" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="AW19" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="AX19" s="6">
         <v>0.9</v>
       </c>
     </row>
-    <row r="20" spans="1:50" ht="15.75" customHeight="1">
+    <row r="20" spans="1:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>81</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>38</v>
@@ -4718,705 +4687,1049 @@
       <c r="T20" s="6">
         <v>0.3</v>
       </c>
-      <c r="W20" s="6" t="s">
-        <v>23</v>
+      <c r="W20" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="X20" s="6">
-        <v>1</v>
-      </c>
-      <c r="Y20" s="7" t="s">
-        <v>13</v>
+        <v>0.12</v>
+      </c>
+      <c r="Y20" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="Z20" s="6">
-        <v>0.12</v>
+        <v>0.38</v>
       </c>
       <c r="AA20" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AB20" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="AC20" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD20" s="6">
+        <v>-1</v>
+      </c>
+      <c r="AE20" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF20" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="AG20" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH20" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="AI20" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ20" s="6">
+        <v>0.72</v>
+      </c>
+      <c r="AK20" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL20" s="6">
         <v>0.38</v>
       </c>
-      <c r="AC20" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD20" s="6">
-        <v>0.3</v>
-      </c>
-      <c r="AE20" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AF20" s="6">
-        <v>-1</v>
-      </c>
-      <c r="AG20" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH20" s="6">
-        <v>0.9</v>
-      </c>
-      <c r="AI20" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AJ20" s="6">
-        <v>0.6</v>
-      </c>
-      <c r="AK20" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AL20" s="6">
-        <v>0.72</v>
-      </c>
       <c r="AM20" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AN20" s="6">
         <v>0.38</v>
       </c>
       <c r="AO20" s="6" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="AP20" s="6">
-        <v>0.38</v>
+        <v>0.62</v>
       </c>
       <c r="AQ20" s="6" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="AR20" s="6">
-        <v>0.62</v>
+        <v>0.3</v>
       </c>
       <c r="AS20" s="6" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="AT20" s="6">
-        <v>0.3</v>
+        <v>0.72</v>
       </c>
       <c r="AU20" s="6" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="AV20" s="6">
-        <v>0.72</v>
-      </c>
-      <c r="AW20" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="AX20" s="6">
         <v>0.9</v>
       </c>
     </row>
-    <row r="21" spans="1:50" ht="15.75" customHeight="1">
+    <row r="21" spans="1:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="W21" s="6" t="s">
-        <v>33</v>
+      <c r="W21" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="X21" s="6">
-        <v>1</v>
-      </c>
-      <c r="Y21" s="7" t="s">
-        <v>13</v>
+        <v>0.82</v>
+      </c>
+      <c r="Y21" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="Z21" s="6">
-        <v>0.82</v>
+        <v>0.9</v>
       </c>
       <c r="AA21" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AB21" s="6">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="AC21" s="2" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="AD21" s="6">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AE21" s="2" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="AF21" s="6">
+        <v>-0.6</v>
+      </c>
+      <c r="AG21" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH21" s="6">
         <v>-1</v>
       </c>
-      <c r="AG21" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH21" s="6">
-        <v>-0.6</v>
-      </c>
       <c r="AI21" s="2" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="AJ21" s="6">
-        <v>-1</v>
-      </c>
-      <c r="AK21" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AL21" s="6">
         <v>-0.8</v>
       </c>
     </row>
-    <row r="22" spans="1:50" ht="15.75" customHeight="1">
+    <row r="22" spans="1:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="W22" s="6" t="s">
-        <v>86</v>
+      <c r="W22" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="X22" s="6">
-        <v>1</v>
-      </c>
-      <c r="Y22" s="7" t="s">
-        <v>13</v>
+        <v>0.75</v>
+      </c>
+      <c r="Y22" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="Z22" s="6">
-        <v>0.75</v>
+        <v>0.91</v>
       </c>
       <c r="AA22" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AB22" s="6">
-        <v>0.91</v>
+        <v>0.61</v>
       </c>
       <c r="AC22" s="2" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="AD22" s="6">
-        <v>0.61</v>
+        <v>-1</v>
       </c>
       <c r="AE22" s="2" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="AF22" s="6">
+        <v>-0.4</v>
+      </c>
+      <c r="AG22" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH22" s="6">
         <v>-1</v>
       </c>
-      <c r="AG22" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH22" s="6">
-        <v>-0.4</v>
-      </c>
       <c r="AI22" s="2" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="AJ22" s="6">
-        <v>-1</v>
-      </c>
-      <c r="AK22" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AL22" s="6">
         <v>-0.85</v>
       </c>
     </row>
-    <row r="23" spans="1:50" ht="15.75" customHeight="1">
+    <row r="23" spans="1:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>58</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="W23" s="6" t="s">
-        <v>55</v>
+      <c r="W23" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="X23" s="6">
-        <v>1</v>
-      </c>
-      <c r="Y23" s="7" t="s">
-        <v>13</v>
+        <v>0.01</v>
+      </c>
+      <c r="Y23" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="Z23" s="6">
-        <v>0.01</v>
+        <v>-0.74</v>
       </c>
       <c r="AA23" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AB23" s="6">
-        <v>-0.74</v>
+        <v>0.85</v>
       </c>
       <c r="AC23" s="2" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="AD23" s="6">
-        <v>0.85</v>
+        <v>-1</v>
       </c>
       <c r="AE23" s="2" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="AF23" s="6">
+        <v>-0.1</v>
+      </c>
+      <c r="AG23" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH23" s="6">
         <v>-1</v>
       </c>
-      <c r="AG23" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH23" s="6">
-        <v>-0.1</v>
-      </c>
       <c r="AI23" s="2" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="AJ23" s="6">
-        <v>-1</v>
-      </c>
-      <c r="AK23" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AL23" s="6">
         <v>0.9</v>
       </c>
     </row>
-    <row r="24" spans="1:50" ht="15.75" customHeight="1">
+    <row r="24" spans="1:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="W24" s="6" t="s">
-        <v>87</v>
+      <c r="W24" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="X24" s="6">
-        <v>1</v>
-      </c>
-      <c r="Y24" s="7" t="s">
-        <v>13</v>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="Y24" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="Z24" s="6">
-        <v>0.28999999999999998</v>
+        <v>0.2</v>
       </c>
       <c r="AA24" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AB24" s="6">
-        <v>0.2</v>
+        <v>0.9</v>
       </c>
       <c r="AC24" s="2" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="AD24" s="6">
-        <v>0.9</v>
+        <v>-1</v>
       </c>
       <c r="AE24" s="2" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="AF24" s="6">
+        <v>-0.2</v>
+      </c>
+      <c r="AG24" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH24" s="6">
         <v>-1</v>
       </c>
-      <c r="AG24" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH24" s="6">
-        <v>-0.2</v>
-      </c>
       <c r="AI24" s="2" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="AJ24" s="6">
-        <v>-1</v>
-      </c>
-      <c r="AK24" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AL24" s="6">
         <v>0.42</v>
       </c>
     </row>
-    <row r="25" spans="1:50" ht="15.75" customHeight="1">
+    <row r="25" spans="1:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>59</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="W25" s="6" t="s">
-        <v>87</v>
+      <c r="W25" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="X25" s="6">
-        <v>1</v>
-      </c>
-      <c r="Y25" s="7" t="s">
-        <v>13</v>
+        <v>-0.4</v>
+      </c>
+      <c r="Y25" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="Z25" s="6">
-        <v>-0.4</v>
+        <v>-0.48</v>
       </c>
       <c r="AA25" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AB25" s="6">
-        <v>-0.48</v>
+        <v>0.84</v>
       </c>
       <c r="AC25" s="2" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="AD25" s="6">
-        <v>0.84</v>
+        <v>-1</v>
       </c>
       <c r="AE25" s="2" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="AF25" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="AG25" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH25" s="6">
         <v>-1</v>
       </c>
-      <c r="AG25" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH25" s="6">
-        <v>0.1</v>
-      </c>
       <c r="AI25" s="2" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="AJ25" s="6">
-        <v>-1</v>
-      </c>
-      <c r="AK25" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AL25" s="6">
         <v>0.73</v>
       </c>
     </row>
-    <row r="26" spans="1:50" ht="15.75" customHeight="1">
+    <row r="26" spans="1:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>84</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="W26" s="6" t="s">
-        <v>23</v>
+      <c r="W26" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="X26" s="6">
-        <v>1</v>
-      </c>
-      <c r="Y26" s="7" t="s">
-        <v>13</v>
+        <v>-0.55000000000000004</v>
+      </c>
+      <c r="Y26" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="Z26" s="6">
-        <v>-0.55000000000000004</v>
+        <v>-0.5</v>
       </c>
       <c r="AA26" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AB26" s="6">
-        <v>-0.5</v>
+        <v>-0.1</v>
       </c>
       <c r="AC26" s="2" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="AD26" s="6">
-        <v>-0.1</v>
+        <v>-1</v>
       </c>
       <c r="AE26" s="2" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="AF26" s="6">
-        <v>-1</v>
+        <v>0.91</v>
       </c>
       <c r="AG26" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AH26" s="6">
-        <v>0.91</v>
+        <v>0.72</v>
       </c>
       <c r="AI26" s="2" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="AJ26" s="6">
-        <v>0.72</v>
-      </c>
-      <c r="AK26" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AL26" s="6">
         <v>0.78</v>
       </c>
     </row>
-    <row r="27" spans="1:50" ht="15.75" customHeight="1">
+    <row r="27" spans="1:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="W27" s="6" t="s">
-        <v>86</v>
+      <c r="W27" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="X27" s="6">
-        <v>1</v>
-      </c>
-      <c r="Y27" s="7" t="s">
-        <v>13</v>
+        <v>0.75</v>
+      </c>
+      <c r="Y27" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="Z27" s="6">
-        <v>0.75</v>
+        <v>0.99</v>
       </c>
       <c r="AA27" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AB27" s="6">
-        <v>0.99</v>
+        <v>0.9</v>
       </c>
       <c r="AC27" s="2" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="AD27" s="6">
-        <v>0.9</v>
+        <v>-1</v>
       </c>
       <c r="AE27" s="2" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="AF27" s="6">
+        <v>-0.65</v>
+      </c>
+      <c r="AG27" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH27" s="6">
         <v>-1</v>
       </c>
-      <c r="AG27" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH27" s="6">
-        <v>-0.65</v>
-      </c>
       <c r="AI27" s="2" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="AJ27" s="6">
-        <v>-1</v>
-      </c>
-      <c r="AK27" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AL27" s="6">
         <v>-0.6</v>
       </c>
     </row>
-    <row r="28" spans="1:50" ht="15.75" customHeight="1">
+    <row r="28" spans="1:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>51</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="W28" s="6" t="s">
-        <v>55</v>
+      <c r="W28" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="X28" s="6">
-        <v>1</v>
-      </c>
-      <c r="Y28" s="7" t="s">
-        <v>13</v>
+        <v>-0.69</v>
+      </c>
+      <c r="Y28" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="Z28" s="6">
-        <v>-0.69</v>
+        <v>-0.85</v>
       </c>
       <c r="AA28" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AB28" s="6">
-        <v>-0.85</v>
+        <v>0.74</v>
       </c>
       <c r="AC28" s="2" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="AD28" s="6">
-        <v>0.74</v>
+        <v>-1</v>
       </c>
       <c r="AE28" s="2" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="AF28" s="6">
+        <v>0.42</v>
+      </c>
+      <c r="AG28" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH28" s="6">
         <v>-1</v>
       </c>
-      <c r="AG28" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH28" s="6">
-        <v>0.42</v>
-      </c>
       <c r="AI28" s="2" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="AJ28" s="6">
-        <v>-1</v>
-      </c>
-      <c r="AK28" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AL28" s="6">
         <v>0.98</v>
       </c>
     </row>
-    <row r="29" spans="1:50" ht="15.75" customHeight="1">
+    <row r="29" spans="1:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>88</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="W29" s="6" t="s">
-        <v>89</v>
+      <c r="W29" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="X29" s="6">
+        <v>-0.56999999999999995</v>
+      </c>
+      <c r="Y29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z29" s="6">
+        <v>-0.69</v>
+      </c>
+      <c r="AA29" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB29" s="6">
+        <v>-0.4</v>
+      </c>
+      <c r="AC29" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD29" s="6">
+        <v>-1</v>
+      </c>
+      <c r="AE29" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF29" s="6">
+        <v>0.98</v>
+      </c>
+      <c r="AG29" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH29" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="AI29" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ29" s="6">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="W30" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="X30" s="6">
+        <v>-0.88</v>
+      </c>
+      <c r="Y30" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z30" s="6">
+        <v>-0.9</v>
+      </c>
+      <c r="AA30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB30" s="6">
+        <v>-0.95</v>
+      </c>
+      <c r="AC30" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD30" s="6">
         <v>1</v>
       </c>
-      <c r="Y29" s="7" t="s">
+      <c r="AE30" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF30" s="6">
+        <v>-0.75</v>
+      </c>
+      <c r="AG30" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH30" s="6">
+        <v>-1</v>
+      </c>
+      <c r="AI30" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ30" s="6">
+        <v>1</v>
+      </c>
+      <c r="AK30" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL30" s="6">
+        <v>-0.9</v>
+      </c>
+      <c r="AM30" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AN30" s="6">
+        <v>-0.9</v>
+      </c>
+      <c r="AO30" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AP30" s="6">
+        <v>0.89</v>
+      </c>
+      <c r="AQ30" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AR30" s="6">
+        <v>-0.95</v>
+      </c>
+      <c r="AS30" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="AT30" s="6">
+        <v>1</v>
+      </c>
+      <c r="AU30" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="AV30" s="6">
+        <v>-0.35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="W31" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="Z29" s="6">
-        <v>-0.56999999999999995</v>
-      </c>
-      <c r="AA29" s="2" t="s">
+      <c r="X31" s="6">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="Y31" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="AB29" s="6">
-        <v>-0.69</v>
-      </c>
-      <c r="AC29" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD29" s="6">
-        <v>-0.4</v>
-      </c>
-      <c r="AE29" s="2" t="s">
+      <c r="Z31" s="6">
+        <v>0.81</v>
+      </c>
+      <c r="AA31" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB31" s="6">
+        <v>0.88</v>
+      </c>
+      <c r="AC31" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="AF29" s="6">
+      <c r="AD31" s="6">
         <v>-1</v>
       </c>
-      <c r="AG29" s="2" t="s">
+      <c r="AE31" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="AH29" s="6">
-        <v>0.98</v>
-      </c>
-      <c r="AI29" s="2" t="s">
+      <c r="AF31" s="6">
+        <v>-0.74</v>
+      </c>
+      <c r="AG31" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="AJ29" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="AK29" s="2" t="s">
+      <c r="AH31" s="6">
+        <v>0.42</v>
+      </c>
+      <c r="AI31" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AL29" s="6">
-        <v>0.72</v>
-      </c>
-    </row>
-    <row r="30" spans="1:50" ht="15.75" customHeight="1">
-      <c r="A30" s="7" t="s">
+      <c r="AJ31" s="6">
+        <v>-0.55000000000000004</v>
+      </c>
+      <c r="AK31" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL31" s="6">
+        <v>0.81</v>
+      </c>
+      <c r="AM31" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AN31" s="6">
+        <v>0.81</v>
+      </c>
+      <c r="AO31" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AP31" s="6">
+        <v>-0.45</v>
+      </c>
+      <c r="AQ31" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AR31" s="6">
+        <v>0.88</v>
+      </c>
+      <c r="AS31" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="AT31" s="6">
+        <v>-0.55000000000000004</v>
+      </c>
+      <c r="AU31" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="AV31" s="6">
+        <v>-0.74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="W32" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="X32" s="6">
+        <v>-0.88</v>
+      </c>
+      <c r="Y32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z32" s="6">
+        <v>-0.9</v>
+      </c>
+      <c r="AA32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB32" s="6">
+        <v>-0.15</v>
+      </c>
+      <c r="AC32" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD32" s="6">
+        <v>0.35</v>
+      </c>
+      <c r="AE32" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF32" s="6">
+        <v>-0.25</v>
+      </c>
+      <c r="AG32" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH32" s="6">
+        <v>-0.75</v>
+      </c>
+      <c r="AI32" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ32" s="6">
+        <v>1</v>
+      </c>
+      <c r="AK32" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL32" s="6">
+        <v>-0.9</v>
+      </c>
+      <c r="AM32" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AN32" s="6">
+        <v>-0.9</v>
+      </c>
+      <c r="AO32" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AP32" s="6">
+        <v>0.89</v>
+      </c>
+      <c r="AQ32" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AR32" s="6">
+        <v>-0.15</v>
+      </c>
+      <c r="AS32" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="AT32" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="AU32" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="AV32" s="6">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="W33" s="7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="31" spans="1:50" ht="15.75" customHeight="1">
-      <c r="A31" s="2" t="s">
+      <c r="X33" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="Y33" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="Z33" s="6">
+        <v>0.87</v>
+      </c>
+      <c r="AA33" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB33" s="6">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="AC33" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD33" s="6">
+        <v>-1</v>
+      </c>
+      <c r="AE33" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF33" s="6">
+        <v>-0.28999999999999998</v>
+      </c>
+      <c r="AG33" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH33" s="6">
+        <v>-1</v>
+      </c>
+      <c r="AI33" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ33" s="6">
+        <v>-0.79</v>
+      </c>
+      <c r="AK33" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL33" s="6">
+        <v>0.87</v>
+      </c>
+      <c r="AM33" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AN33" s="6">
+        <v>0.87</v>
+      </c>
+      <c r="AO33" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AP33" s="6">
+        <v>-0.59</v>
+      </c>
+      <c r="AQ33" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AR33" s="6">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="AS33" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="AT33" s="6">
+        <v>-0.79</v>
+      </c>
+      <c r="AU33" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="AV33" s="6">
+        <v>-0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="W34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="X34" s="6">
+        <v>-0.8</v>
+      </c>
+      <c r="Y34" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="32" spans="1:50" ht="15.75" customHeight="1">
-      <c r="A32" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A33" s="2" t="s">
+      <c r="Z34" s="6">
+        <v>-0.75</v>
+      </c>
+      <c r="AA34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB34" s="6">
+        <v>-0.95</v>
+      </c>
+      <c r="AC34" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="AD34" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE34" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF34" s="6">
+        <v>-0.49</v>
+      </c>
+      <c r="AG34" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH34" s="6">
+        <v>-0.8</v>
+      </c>
+      <c r="AI34" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ34" s="6">
+        <v>0.87</v>
+      </c>
+      <c r="AK34" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL34" s="6">
+        <v>-0.7</v>
+      </c>
+      <c r="AM34" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AN34" s="6">
+        <v>-0.7</v>
+      </c>
+      <c r="AO34" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AP34" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="AQ34" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AR34" s="6">
+        <v>0.68</v>
+      </c>
+      <c r="AS34" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="AT34" s="6">
+        <v>0.85</v>
+      </c>
+      <c r="AU34" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="AV34" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="W35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="X35" s="6">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="Y35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z35" s="6">
+        <v>0.81</v>
+      </c>
+      <c r="AA35" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB35" s="6">
+        <v>0.88</v>
+      </c>
+      <c r="AC35" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A34" s="2" t="s">
+      <c r="AD35" s="6">
+        <v>-1</v>
+      </c>
+      <c r="AE35" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A35" s="2" t="s">
+      <c r="AF35" s="6">
+        <v>-0.74</v>
+      </c>
+      <c r="AG35" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A36" s="2" t="s">
+      <c r="AH35" s="6">
+        <v>0.42</v>
+      </c>
+      <c r="AI35" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A37" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A38" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A39" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A40" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A41" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A42" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A43" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>89</v>
+      <c r="AJ35" s="6">
+        <v>-0.55000000000000004</v>
+      </c>
+      <c r="AK35" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL35" s="6">
+        <v>0.81</v>
+      </c>
+      <c r="AM35" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AN35" s="6">
+        <v>0.81</v>
+      </c>
+      <c r="AO35" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AP35" s="6">
+        <v>-0.45</v>
+      </c>
+      <c r="AQ35" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AR35" s="6">
+        <v>0.88</v>
+      </c>
+      <c r="AS35" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="AT35" s="6">
+        <v>-0.55000000000000004</v>
+      </c>
+      <c r="AU35" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="AV35" s="6">
+        <v>-0.74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>